<commit_message>
combine two excel files into 1
</commit_message>
<xml_diff>
--- a/datas/schedule.xlsx
+++ b/datas/schedule.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\important\interesting python projects\zoom_reminder\Class-reminder\datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F846321-3415-4B5E-B0DA-D28BBE213151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD195539-D484-43CB-A21F-4C32F74C01B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17496" yWindow="0" windowWidth="21600" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="schedule" sheetId="1" r:id="rId1"/>
+    <sheet name="desc" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t>start_time</t>
   </si>
@@ -33,9 +34,6 @@
     <t>L10</t>
   </si>
   <si>
-    <t>DD1</t>
-  </si>
-  <si>
     <t>T1</t>
   </si>
   <si>
@@ -67,6 +65,114 @@
   </si>
   <si>
     <t>Td3</t>
+  </si>
+  <si>
+    <t>Đ1</t>
+  </si>
+  <si>
+    <t>Tin Học</t>
+  </si>
+  <si>
+    <t>Bùi Tiến Dũng</t>
+  </si>
+  <si>
+    <t>thaymanhdz</t>
+  </si>
+  <si>
+    <t>Quốc Phòng</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Mạnh</t>
+  </si>
+  <si>
+    <t>Thể dục</t>
+  </si>
+  <si>
+    <t>Trần Mạnh Hùng</t>
+  </si>
+  <si>
+    <t>huong24</t>
+  </si>
+  <si>
+    <t>Lịch Sử</t>
+  </si>
+  <si>
+    <t>Nguyễn Thu Hương</t>
+  </si>
+  <si>
+    <t>Sinh Học</t>
+  </si>
+  <si>
+    <t>Huỳnh Thị Ái Tâm</t>
+  </si>
+  <si>
+    <t>Hoahoc11</t>
+  </si>
+  <si>
+    <t>Hóa Học</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Thu Cúc</t>
+  </si>
+  <si>
+    <t>Công Nghệ</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Quảng</t>
+  </si>
+  <si>
+    <t>Tiếng Anh</t>
+  </si>
+  <si>
+    <t>Mai Thành Sơn</t>
+  </si>
+  <si>
+    <t>Giáo dục công dân</t>
+  </si>
+  <si>
+    <t>Trần Văn Năng</t>
+  </si>
+  <si>
+    <t>Địa Lý</t>
+  </si>
+  <si>
+    <t>Nguyễn Mạnh Hà</t>
+  </si>
+  <si>
+    <t>Ngữ Văn</t>
+  </si>
+  <si>
+    <t>Khương Thị Thu Cúc</t>
+  </si>
+  <si>
+    <t>Covid-19</t>
+  </si>
+  <si>
+    <t>Toán</t>
+  </si>
+  <si>
+    <t>Hạ Vũ Anh</t>
+  </si>
+  <si>
+    <t>Vật Lý</t>
+  </si>
+  <si>
+    <t>Triệu Lê Quang</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>TEACHER</t>
   </si>
 </sst>
 </file>
@@ -391,7 +497,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,19 +536,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -456,16 +562,16 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -479,16 +585,16 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -496,19 +602,19 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
         <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -516,19 +622,19 @@
         <v>0.4513888888888889</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -536,7 +642,7 @@
         <v>0.57291666666666663</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -544,7 +650,7 @@
         <v>0.60763888888888895</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -552,7 +658,7 @@
         <v>0.64236111111111105</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -564,4 +670,257 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6926B7ED-0870-4C01-B36A-8876AC994FF9}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>3141537349</v>
+      </c>
+      <c r="E2">
+        <v>994494</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>8258073057</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>9765088770</v>
+      </c>
+      <c r="E4">
+        <v>614989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>6822045197</v>
+      </c>
+      <c r="E5">
+        <v>1234567890</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>8856018255</v>
+      </c>
+      <c r="E6">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>2655252337</v>
+      </c>
+      <c r="E7">
+        <v>91089</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>7361311308</v>
+      </c>
+      <c r="E8">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>5841603699</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>7174188443</v>
+      </c>
+      <c r="E10">
+        <v>66886868</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>7666693318</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>5678955431</v>
+      </c>
+      <c r="E12">
+        <v>989938</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>9102597428</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>2066767262</v>
+      </c>
+      <c r="E14">
+        <v>123456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>